<commit_message>
Added bar codes and recovery dates where necessary
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP02PMCI_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_CP02PMCI_00001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\# OOI_Asset_Management\CP_mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
     <definedName name="_FilterDatabase_1_1_1_1_1_1">Moorings!$B$1:$K$102</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$H$406</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="75">
   <si>
     <t>Ref Des</t>
   </si>
@@ -246,9 +246,6 @@
     <t>CP02PMCI-WFP01-00-WFPENG000</t>
   </si>
   <si>
-    <t>This serial number is a placekeeper used until the correct serial number is found or defined</t>
-  </si>
-  <si>
     <t>Mooring OOIBARCODE</t>
   </si>
   <si>
@@ -283,6 +280,12 @@
   </si>
   <si>
     <t>ML13103-02</t>
+  </si>
+  <si>
+    <t>OL000339</t>
+  </si>
+  <si>
+    <t>OL000239</t>
   </si>
 </sst>
 </file>
@@ -384,11 +387,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
@@ -427,6 +425,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -779,13 +783,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -829,25 +833,25 @@
     <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="298">
@@ -1521,7 +1525,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,46 +1542,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="21" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>10</v>
@@ -1610,8 +1614,14 @@
         <v>55</v>
       </c>
       <c r="L2" s="12"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
+      <c r="M2" s="22">
+        <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="N",1,-1))</f>
+        <v>40.226649999999999</v>
+      </c>
+      <c r="N2" s="22">
+        <f>((LEFT(I2,(FIND("°",I2,1)-1)))+(MID(I2,(FIND("°",I2,1)+1),(FIND("'",I2,1))-(FIND("°",I2,1)+1))/60))*(IF(RIGHT(I2,1)="E",1,-1))</f>
+        <v>-70.88858333333333</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1629,7 +1639,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1650,7 +1660,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>12</v>
@@ -1659,7 +1669,7 @@
         <v>39</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>13</v>
@@ -1679,16 +1689,16 @@
         <v>58</v>
       </c>
       <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>64</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>65</v>
       </c>
       <c r="F2" s="2">
         <v>18596</v>
@@ -1708,16 +1718,16 @@
         <v>58</v>
       </c>
       <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>64</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>65</v>
       </c>
       <c r="F3" s="2">
         <v>18596</v>
@@ -1734,16 +1744,16 @@
         <v>58</v>
       </c>
       <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>64</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>65</v>
       </c>
       <c r="F4" s="2">
         <v>18596</v>
@@ -1766,7 +1776,7 @@
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
@@ -1774,7 +1784,9 @@
       <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
       <c r="F6" s="2" t="s">
         <v>40</v>
       </c>
@@ -1793,7 +1805,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>11</v>
@@ -1802,10 +1814,10 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" t="s">
         <v>66</v>
-      </c>
-      <c r="F8" t="s">
-        <v>67</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>17</v>
@@ -1822,7 +1834,7 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>11</v>
@@ -1831,10 +1843,10 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
         <v>66</v>
-      </c>
-      <c r="F9" t="s">
-        <v>67</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>18</v>
@@ -1848,7 +1860,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>11</v>
@@ -1857,10 +1869,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" t="s">
         <v>66</v>
-      </c>
-      <c r="F10" t="s">
-        <v>67</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>20</v>
@@ -1874,7 +1886,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>11</v>
@@ -1883,10 +1895,10 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" t="s">
         <v>66</v>
-      </c>
-      <c r="F11" t="s">
-        <v>67</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>21</v>
@@ -1900,7 +1912,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>11</v>
@@ -1909,10 +1921,10 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
         <v>66</v>
-      </c>
-      <c r="F12" t="s">
-        <v>67</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>22</v>
@@ -1926,7 +1938,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
@@ -1935,10 +1947,10 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" t="s">
         <v>66</v>
-      </c>
-      <c r="F13" t="s">
-        <v>67</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>23</v>
@@ -1952,7 +1964,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
@@ -1961,10 +1973,10 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="s">
         <v>66</v>
-      </c>
-      <c r="F14" t="s">
-        <v>67</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>24</v>
@@ -1978,7 +1990,7 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>11</v>
@@ -1987,10 +1999,10 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" t="s">
         <v>66</v>
-      </c>
-      <c r="F15" t="s">
-        <v>67</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>25</v>
@@ -2010,7 +2022,7 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>11</v>
@@ -2019,7 +2031,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F17" s="6">
         <v>125</v>
@@ -2039,7 +2051,7 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>11</v>
@@ -2048,7 +2060,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F18" s="6">
         <v>125</v>
@@ -2071,7 +2083,7 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>11</v>
@@ -2080,7 +2092,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F20" s="1">
         <v>100037</v>
@@ -2100,7 +2112,7 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>11</v>
@@ -2109,7 +2121,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F21" s="1">
         <v>100037</v>
@@ -2131,7 +2143,7 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>11</v>
@@ -2140,7 +2152,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F23" s="6">
         <v>1119</v>
@@ -2160,7 +2172,7 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>11</v>
@@ -2169,7 +2181,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F24" s="6">
         <v>1119</v>
@@ -2189,7 +2201,7 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>11</v>
@@ -2198,7 +2210,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F25" s="6">
         <v>1119</v>
@@ -2215,7 +2227,7 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>11</v>
@@ -2224,7 +2236,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F26" s="6">
         <v>1119</v>
@@ -2241,7 +2253,7 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>11</v>
@@ -2250,7 +2262,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F27" s="6">
         <v>1119</v>
@@ -2270,7 +2282,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>11</v>
@@ -2279,7 +2291,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F28" s="6">
         <v>1119</v>
@@ -2296,7 +2308,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>11</v>
@@ -2305,7 +2317,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F29" s="6">
         <v>1119</v>
@@ -2322,7 +2334,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>11</v>
@@ -2331,7 +2343,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F30" s="6">
         <v>1119</v>
@@ -2348,7 +2360,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>11</v>
@@ -2357,7 +2369,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F31" s="6">
         <v>1119</v>
@@ -2374,7 +2386,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>11</v>
@@ -2383,7 +2395,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F32" s="6">
         <v>1119</v>
@@ -2406,7 +2418,7 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>11</v>
@@ -2415,7 +2427,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F34" s="6">
         <v>20465</v>
@@ -2435,7 +2447,7 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>11</v>
@@ -2444,7 +2456,7 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F35" s="6">
         <v>20465</v>
@@ -2468,7 +2480,7 @@
         <v>60</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>11</v>
@@ -2477,10 +2489,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2488,7 +2500,7 @@
         <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>11</v>
@@ -2496,13 +2508,13 @@
       <c r="D39" s="2">
         <v>1</v>
       </c>
-      <c r="E39" s="2"/>
+      <c r="E39" t="s">
+        <v>74</v>
+      </c>
       <c r="F39" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I39" s="20" t="s">
-        <v>61</v>
-      </c>
+      <c r="I39" s="20"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F42" s="6"/>

</xml_diff>